<commit_message>
add filter, enhance report
</commit_message>
<xml_diff>
--- a/Logiz.Radar/wwwroot/template/logiz.radar.test-case.xlsx
+++ b/Logiz.Radar/wwwroot/template/logiz.radar.test-case.xlsx
@@ -163,7 +163,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -186,6 +186,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -467,7 +470,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -483,7 +486,11 @@
     <col min="8" max="8" width="11.90625" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.36328125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="18.1796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="13.6328125" style="2"/>
+    <col min="11" max="13" width="13.6328125" style="2"/>
+    <col min="14" max="14" width="13.6328125" style="10"/>
+    <col min="15" max="15" width="13.6328125" style="2"/>
+    <col min="16" max="16" width="18.1796875" style="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="13.6328125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="29" x14ac:dyDescent="0.35">

</xml_diff>